<commit_message>
changement de la contrainte sur le type du profile 21b5e9a24b0e27135bf3294fa2d98c0a1a43d150
</commit_message>
<xml_diff>
--- a/FL-gt-structure/ig/StructureDefinition-fr-core-organization-etablissement.xlsx
+++ b/FL-gt-structure/ig/StructureDefinition-fr-core-organization-etablissement.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-02T20:15:58+00:00</t>
+    <t>2025-12-02T20:49:48+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -12866,7 +12866,7 @@
         <v>78</v>
       </c>
       <c r="X94" t="s" s="2">
-        <v>257</v>
+        <v>158</v>
       </c>
       <c r="Y94" s="2"/>
       <c r="Z94" t="s" s="2">

</xml_diff>